<commit_message>
Replacing all normal pats and hugs with embeds <3
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Take over</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Pats etc</t>
   </si>
   <si>
-    <t>Add multiple Users as parameter</t>
-  </si>
-  <si>
     <t>Dynamic prefix</t>
   </si>
   <si>
@@ -96,6 +93,12 @@
   </si>
   <si>
     <t>http://git.argus.moe/serenity/SoraBot/wikis/sora-help</t>
+  </si>
+  <si>
+    <t>Add multiple Users as parameter, high5</t>
+  </si>
+  <si>
+    <t>multiple ppl as parameter</t>
   </si>
 </sst>
 </file>
@@ -462,20 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="55.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,112 +487,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supporting multiple mentions on same Interaction. Added punch and high5
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -95,10 +95,10 @@
     <t>http://git.argus.moe/serenity/SoraBot/wikis/sora-help</t>
   </si>
   <si>
-    <t>Add multiple Users as parameter, high5</t>
-  </si>
-  <si>
-    <t>multiple ppl as parameter</t>
+    <t>Dont invoke if the message starts with the Guild's prefix</t>
+  </si>
+  <si>
+    <t>Add multiple Users as parameter, high5, not more then 1 mention of same person</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -479,7 +479,7 @@
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,78 +487,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Finished Dynamic prefixes and adapting the Afk service to it :D
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Take over</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Addition</t>
   </si>
   <si>
-    <t>Pats etc</t>
-  </si>
-  <si>
     <t>Dynamic prefix</t>
   </si>
   <si>
@@ -105,13 +102,52 @@
   </si>
   <si>
     <t xml:space="preserve"> not more then 1 mention of same person</t>
+  </si>
+  <si>
+    <t>Minimum star count per guild setting</t>
+  </si>
+  <si>
+    <t>support divorces with ID only =&gt; even without connection to sora</t>
+  </si>
+  <si>
+    <t>after couple warnings auto actions dont work</t>
+  </si>
+  <si>
+    <t>add reason to official discord log</t>
+  </si>
+  <si>
+    <t>repeat</t>
+  </si>
+  <si>
+    <t>save playlist maybe? VIP ONLY?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marriage limit!!! </t>
+  </si>
+  <si>
+    <t>pagify taglist!</t>
+  </si>
+  <si>
+    <t>purge / clear commands</t>
+  </si>
+  <si>
+    <t>actually make it work now :^)</t>
+  </si>
+  <si>
+    <t>image search?</t>
+  </si>
+  <si>
+    <t>guild doesnt require pic</t>
+  </si>
+  <si>
+    <t>guild doesnt require emojis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +158,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,16 +193,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,14 +521,14 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.28515625" customWidth="1"/>
     <col min="2" max="2" width="55.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -495,122 +542,159 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A23" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Keeps track of given Interactions as well now. Added info module
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Take over</t>
   </si>
@@ -141,13 +141,19 @@
   </si>
   <si>
     <t>guild doesnt require emojis</t>
+  </si>
+  <si>
+    <t>add possibility for owners to make a default join role?</t>
+  </si>
+  <si>
+    <t>Track given interactions aswell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +176,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +196,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,18 +210,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -518,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,9 +566,10 @@
     <col min="2" max="2" width="55.140625" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -553,18 +590,24 @@
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -572,7 +615,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -586,7 +629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -594,12 +637,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -610,7 +653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -618,12 +661,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -631,7 +674,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -642,12 +685,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -666,13 +709,13 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to fix the DB, Taglists
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Take over</t>
   </si>
@@ -147,13 +147,25 @@
   </si>
   <si>
     <t>Track given interactions aswell</t>
+  </si>
+  <si>
+    <t>whitespace check</t>
+  </si>
+  <si>
+    <t>add fileattachment support</t>
+  </si>
+  <si>
+    <t>change emote next to affinity to display affinity</t>
+  </si>
+  <si>
+    <t>Sentry service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,8 +195,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +218,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -226,22 +250,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Link" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,9 +594,10 @@
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -593,13 +621,16 @@
       <c r="E3" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -607,7 +638,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -615,7 +646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -629,7 +660,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -637,12 +668,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -653,7 +684,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -661,20 +692,26 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -685,12 +722,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -727,6 +764,11 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completing the tag service
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Take over</t>
   </si>
@@ -159,13 +160,40 @@
   </si>
   <si>
     <t>Sentry service</t>
+  </si>
+  <si>
+    <t>ADD Ids TO SHIT</t>
+  </si>
+  <si>
+    <t>fix how sora fails</t>
+  </si>
+  <si>
+    <t>if there is 1 link to 1 image embed it aswell</t>
+  </si>
+  <si>
+    <t>hug group =&gt; sora hugs u instead</t>
+  </si>
+  <si>
+    <t>permissions / role setup</t>
+  </si>
+  <si>
+    <t>implement better dependency injection</t>
+  </si>
+  <si>
+    <t>1. https://github.com/foxbot/patek/blob/master/src/Patek/Services/CommandHandlingService.cs</t>
+  </si>
+  <si>
+    <t>2. https://github.com/foxbot/patek/blob/master/src/Patek/Program.cs#L46</t>
+  </si>
+  <si>
+    <t>3. https://github.com/foxbot/patek/blob/master/src/Patek/Program.cs#L31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +209,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -188,22 +223,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,11 +239,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -250,25 +266,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
+  <cellStyles count="4">
+    <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
+    <cellStyle name="Link" xfId="3" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,9 +610,10 @@
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -624,13 +640,16 @@
       <c r="F3" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -638,7 +657,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -646,7 +665,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -660,7 +679,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -668,12 +687,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -684,7 +703,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -692,26 +711,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -722,12 +747,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -735,18 +760,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -755,31 +780,60 @@
       <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A23" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId1" tooltip="https://github.com/foxbot/patek/blob/master/src/Patek/Services/CommandHandlingService.cs" display="https://github.com/foxbot/patek/blob/master/src/Patek/Services/CommandHandlingService.cs"/>
+    <hyperlink ref="B26" r:id="rId2" location="L46" tooltip="https://github.com/foxbot/patek/blob/master/src/Patek/Program.cs#L46" display="https://github.com/foxbot/patek/blob/master/src/Patek/Program.cs - L46"/>
+    <hyperlink ref="B27" r:id="rId3" location="L31" tooltip="https://github.com/foxbot/patek/blob/master/src/Patek/Program.cs#L31" display="https://github.com/foxbot/patek/blob/master/src/Patek/Program.cs - L31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added fun and misc modules
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Take over</t>
   </si>
@@ -187,6 +186,9 @@
   </si>
   <si>
     <t>3. https://github.com/foxbot/patek/blob/master/src/Patek/Program.cs#L31</t>
+  </si>
+  <si>
+    <t>DONT CREATE SORA ROLE TWICE</t>
   </si>
 </sst>
 </file>
@@ -599,7 +601,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,6 +737,9 @@
       <c r="F13" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
Completed the Profilecard, ep Service
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Take over</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>DONT CREATE SORA ROLE TWICE</t>
+  </si>
+  <si>
+    <t>add attachment to the setbg</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,8 +769,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,12 +791,12 @@
       <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nearly completed Music service just to realize discord.net lib has a memory leak and so i could scrap it completely ♥
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -604,7 +604,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +698,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">

</xml_diff>

<commit_message>
Added anime, manga and Character search as well as sentry service ;)
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Take over</t>
   </si>
@@ -192,13 +192,16 @@
   </si>
   <si>
     <t>add attachment to the setbg</t>
+  </si>
+  <si>
+    <t>maybe prefix is null?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +231,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +254,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -271,24 +286,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Link" xfId="3" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,7 +622,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,6 +671,9 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -685,7 +706,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -806,7 +827,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
aded weather and thus completed all the searches!
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -233,7 +233,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,7 +258,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -306,7 +306,7 @@
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Link" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
+    <cellStyle name="Schlecht" xfId="4" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,10 +706,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make DB Threadsafe, Added Reminders and they actually work not like in sora v1 kek
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -622,7 +622,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,10 +684,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started marriages, made custom affinity emotes
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Take over</t>
   </si>
@@ -195,13 +195,16 @@
   </si>
   <si>
     <t>maybe prefix is null?</t>
+  </si>
+  <si>
+    <t>auto role</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +241,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +269,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -286,14 +301,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -301,11 +317,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Link" xfId="3" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="4" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -622,7 +640,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +689,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -704,6 +722,9 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -766,7 +787,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">

</xml_diff>

<commit_message>
fucking fixed the marriages but still getting errors but its working so its fine fuck the rest
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -204,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,15 +241,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,11 +262,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -301,15 +289,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -317,13 +304,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Link" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="4" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -640,7 +625,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,13 +772,13 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
this is how a mental breakdown looks likes. DB wipe, complete rewrite of db mechanics. new way of dependency injection and many manly tears
</commit_message>
<xml_diff>
--- a/SoraBot-v2/To-Do List.xlsx
+++ b/SoraBot-v2/To-Do List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Take over</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>auto role</t>
+  </si>
+  <si>
+    <t>dont marry bots</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,6 +784,9 @@
       <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>